<commit_message>
dodano programy w matlabie
</commit_message>
<xml_diff>
--- a/lengthTest/ch130zbiorczy.xlsx
+++ b/lengthTest/ch130zbiorczy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mikol\Desktop\tabu_search2\lengthTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F923861-E9C7-490D-9FB5-50B292E409B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7031F6DA-A286-4F1D-9601-835542639079}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11169,16 +11169,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>335282</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>174172</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>182881</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>87087</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>315687</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>76201</xdr:rowOff>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>163286</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>174173</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -11471,8 +11471,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AC299"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AB1" sqref="AB1:AC299"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AE16" sqref="AE16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>